<commit_message>
Implemented 100x100 map and fixed last column bug
</commit_message>
<xml_diff>
--- a/BoGmap.xlsx
+++ b/BoGmap.xlsx
@@ -1021,7 +1021,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1031,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DW5891"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AV54" sqref="AV54"/>
+    <sheetView tabSelected="1" topLeftCell="D49" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AS27" sqref="AS27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
World map XML conversion
</commit_message>
<xml_diff>
--- a/BoGmap.xlsx
+++ b/BoGmap.xlsx
@@ -18,8 +18,16 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="world" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="D:\Users\Jesse\Documents\Private\Original\BaneOfGluttony\src\XML\world.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10028" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10028" uniqueCount="140">
   <si>
     <t>M</t>
   </si>
@@ -367,9 +375,6 @@
   </si>
   <si>
     <t>P - You find another outpost. This one has nothing but a signpost and empty guardhouse. Before it is a sign. "On lunch break. Farmlands to the east. Savanna to the west. Beware ye beasts, yadda yadda."</t>
-  </si>
-  <si>
-    <t>Fa - Blcok</t>
   </si>
   <si>
     <t>R - block</t>
@@ -1031,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DW5891"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D49" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AS27" sqref="AS27"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5699,7 +5704,7 @@
         <v>81</v>
       </c>
       <c r="AB16" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AC16" s="22" t="s">
         <v>17</v>
@@ -5998,10 +6003,10 @@
         <v>81</v>
       </c>
       <c r="Z17" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA17" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AB17" s="22" t="s">
         <v>17</v>
@@ -6303,7 +6308,7 @@
         <v>81</v>
       </c>
       <c r="Z18" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA18" s="21" t="s">
         <v>17</v>
@@ -6605,7 +6610,7 @@
         <v>17</v>
       </c>
       <c r="Y19" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Z19" s="21" t="s">
         <v>17</v>
@@ -7676,19 +7681,19 @@
         <v>81</v>
       </c>
       <c r="BY22" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BZ22" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CA22" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CB22" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CC22" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CD22" s="9" t="s">
         <v>105</v>
@@ -7957,13 +7962,13 @@
         <v>81</v>
       </c>
       <c r="BQ23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BR23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BS23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BT23" s="19" t="s">
         <v>81</v>
@@ -7975,25 +7980,25 @@
         <v>81</v>
       </c>
       <c r="BW23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BX23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BY23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BZ23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CA23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CB23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CC23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CD23" s="9" t="s">
         <v>105</v>
@@ -8253,52 +8258,52 @@
         <v>0</v>
       </c>
       <c r="BN24" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BO24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BP24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BQ24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BR24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BS24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BT24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BU24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BV24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BW24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BX24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BY24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BZ24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CA24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CB24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CC24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CD24" s="9" t="s">
         <v>105</v>
@@ -8319,7 +8324,7 @@
         <v>78</v>
       </c>
       <c r="CJ24" s="52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="CK24" s="19" t="s">
         <v>3</v>
@@ -8573,46 +8578,46 @@
         <v>18</v>
       </c>
       <c r="BS25" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BT25" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BU25" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BV25" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BW25" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BX25" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BY25" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BZ25" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CA25" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CB25" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CC25" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CD25" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CE25" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CF25" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CG25" s="15" t="s">
         <v>78</v>
@@ -8621,13 +8626,13 @@
         <v>78</v>
       </c>
       <c r="CI25" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="CJ25" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="CK25" s="52" t="s">
         <v>119</v>
-      </c>
-      <c r="CJ25" s="52" t="s">
-        <v>122</v>
-      </c>
-      <c r="CK25" s="52" t="s">
-        <v>120</v>
       </c>
       <c r="CL25" s="20" t="s">
         <v>83</v>
@@ -8800,16 +8805,16 @@
         <v>17</v>
       </c>
       <c r="AS26" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AT26" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AU26" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AV26" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AW26" s="21" t="s">
         <v>17</v>
@@ -8881,55 +8886,55 @@
         <v>18</v>
       </c>
       <c r="BT26" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BU26" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BV26" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BW26" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BX26" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BY26" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BZ26" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CA26" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CB26" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CC26" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CD26" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CE26" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CF26" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CG26" s="15" t="s">
         <v>78</v>
       </c>
       <c r="CH26" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="CI26" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="CI26" s="52" t="s">
-        <v>120</v>
-      </c>
       <c r="CJ26" s="52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CK26" s="20" t="s">
         <v>83</v>
@@ -9105,7 +9110,7 @@
         <v>17</v>
       </c>
       <c r="AS27" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AT27" s="21" t="s">
         <v>17</v>
@@ -9114,7 +9119,7 @@
         <v>17</v>
       </c>
       <c r="AV27" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AW27" s="21" t="s">
         <v>17</v>
@@ -9189,49 +9194,49 @@
         <v>18</v>
       </c>
       <c r="BU27" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BV27" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BW27" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BX27" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BY27" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BZ27" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CA27" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CB27" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CC27" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CD27" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CE27" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CF27" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CG27" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CH27" s="53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CI27" s="52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CJ27" s="20" t="s">
         <v>1</v>
@@ -9410,16 +9415,16 @@
         <v>17</v>
       </c>
       <c r="AS28" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AT28" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AU28" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AV28" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AW28" s="21" t="s">
         <v>17</v>
@@ -9497,43 +9502,43 @@
         <v>18</v>
       </c>
       <c r="BV28" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BW28" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BX28" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BY28" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BZ28" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CA28" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CB28" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CC28" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CD28" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CE28" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CF28" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CG28" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CH28" s="53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CI28" s="20" t="s">
         <v>1</v>
@@ -9802,40 +9807,40 @@
         <v>18</v>
       </c>
       <c r="BW29" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BX29" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BY29" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ29" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CA29" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CB29" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CC29" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CD29" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CE29" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CF29" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CG29" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CH29" s="53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CI29" s="20" t="s">
         <v>1</v>
@@ -10107,37 +10112,37 @@
         <v>18</v>
       </c>
       <c r="BX30" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BY30" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ30" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CA30" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CB30" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CC30" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CD30" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CE30" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CF30" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CG30" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CH30" s="53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CI30" s="20" t="s">
         <v>1</v>
@@ -10409,40 +10414,40 @@
         <v>18</v>
       </c>
       <c r="BX31" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BY31" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ31" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA31" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CB31" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CC31" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CD31" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CE31" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CF31" s="53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CG31" s="53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CH31" s="53" t="s">
         <v>51</v>
       </c>
       <c r="CI31" s="53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CJ31" s="20" t="s">
         <v>1</v>
@@ -10681,7 +10686,7 @@
         <v>17</v>
       </c>
       <c r="BN32" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="BO32" s="21" t="s">
         <v>17</v>
@@ -10714,37 +10719,37 @@
         <v>18</v>
       </c>
       <c r="BY32" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ32" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CA32" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CB32" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CC32" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="CD32" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CE32" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="CF32" s="53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CG32" s="53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CH32" s="53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CI32" s="53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="CJ32" s="20" t="s">
         <v>1</v>
@@ -11016,7 +11021,7 @@
         <v>18</v>
       </c>
       <c r="BY33" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ33" s="11" t="s">
         <v>18</v>
@@ -11318,7 +11323,7 @@
         <v>18</v>
       </c>
       <c r="BY34" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BZ34" s="11" t="s">
         <v>18</v>
@@ -12669,7 +12674,7 @@
         <v>81</v>
       </c>
       <c r="X39" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y39" s="10" t="s">
         <v>11</v>
@@ -12972,10 +12977,10 @@
         <v>81</v>
       </c>
       <c r="X40" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y40" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z40" s="10" t="s">
         <v>11</v>
@@ -13275,13 +13280,13 @@
         <v>81</v>
       </c>
       <c r="X41" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y41" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z41" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA41" s="10" t="s">
         <v>11</v>
@@ -13305,7 +13310,7 @@
         <v>21</v>
       </c>
       <c r="AH41" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AI41" s="7" t="s">
         <v>21</v>
@@ -13581,13 +13586,13 @@
         <v>81</v>
       </c>
       <c r="Y42" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z42" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA42" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB42" s="10" t="s">
         <v>11</v>
@@ -13883,13 +13888,13 @@
         <v>81</v>
       </c>
       <c r="Y43" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z43" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA43" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB43" s="10" t="s">
         <v>11</v>
@@ -14185,13 +14190,13 @@
         <v>81</v>
       </c>
       <c r="Y44" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z44" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA44" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB44" s="10" t="s">
         <v>11</v>
@@ -14490,10 +14495,10 @@
         <v>81</v>
       </c>
       <c r="Z45" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA45" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB45" s="10" t="s">
         <v>11</v>
@@ -14520,7 +14525,7 @@
         <v>21</v>
       </c>
       <c r="AJ45" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AK45" s="7" t="s">
         <v>21</v>
@@ -14792,13 +14797,13 @@
         <v>81</v>
       </c>
       <c r="Z46" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA46" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB46" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC46" s="10" t="s">
         <v>11</v>
@@ -15094,13 +15099,13 @@
         <v>81</v>
       </c>
       <c r="Z47" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA47" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB47" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC47" s="10" t="s">
         <v>11</v>
@@ -15163,7 +15168,7 @@
         <v>21</v>
       </c>
       <c r="AW47" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AX47" s="17" t="s">
         <v>3</v>
@@ -15396,16 +15401,16 @@
         <v>81</v>
       </c>
       <c r="Z48" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA48" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB48" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC48" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD48" s="10" t="s">
         <v>11</v>
@@ -15465,7 +15470,7 @@
         <v>21</v>
       </c>
       <c r="AW48" s="54" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="AX48" s="19" t="s">
         <v>3</v>
@@ -15701,13 +15706,13 @@
         <v>81</v>
       </c>
       <c r="AA49" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB49" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC49" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD49" s="10" t="s">
         <v>11</v>
@@ -15772,8 +15777,8 @@
       <c r="AX49" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AY49" s="17" t="s">
-        <v>3</v>
+      <c r="AY49" s="41" t="s">
+        <v>19</v>
       </c>
       <c r="AZ49" s="27" t="s">
         <v>8</v>
@@ -16003,13 +16008,13 @@
         <v>81</v>
       </c>
       <c r="AA50" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB50" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC50" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD50" s="10" t="s">
         <v>11</v>
@@ -16305,13 +16310,13 @@
         <v>81</v>
       </c>
       <c r="AA51" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB51" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC51" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD51" s="10" t="s">
         <v>11</v>
@@ -16693,8 +16698,8 @@
       <c r="BC52" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="BD52" s="17" t="s">
-        <v>3</v>
+      <c r="BD52" s="41" t="s">
+        <v>19</v>
       </c>
       <c r="BE52" s="27" t="s">
         <v>8</v>
@@ -16909,13 +16914,13 @@
         <v>81</v>
       </c>
       <c r="AA53" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB53" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC53" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD53" s="11" t="s">
         <v>18</v>
@@ -17208,16 +17213,16 @@
         <v>81</v>
       </c>
       <c r="Z54" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA54" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB54" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC54" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD54" s="11" t="s">
         <v>18</v>
@@ -17510,16 +17515,16 @@
         <v>81</v>
       </c>
       <c r="Z55" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA55" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB55" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC55" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD55" s="11" t="s">
         <v>18</v>
@@ -17812,16 +17817,16 @@
         <v>81</v>
       </c>
       <c r="Z56" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA56" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB56" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC56" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD56" s="11" t="s">
         <v>18</v>
@@ -18111,19 +18116,19 @@
         <v>81</v>
       </c>
       <c r="Y57" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z57" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA57" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB57" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC57" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD57" s="11" t="s">
         <v>18</v>
@@ -18413,19 +18418,19 @@
         <v>81</v>
       </c>
       <c r="Y58" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z58" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA58" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB58" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC58" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD58" s="11" t="s">
         <v>18</v>
@@ -18715,16 +18720,16 @@
         <v>81</v>
       </c>
       <c r="Y59" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z59" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="Z59" s="42" t="s">
-        <v>134</v>
-      </c>
       <c r="AA59" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB59" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC59" s="11" t="s">
         <v>18</v>
@@ -19017,16 +19022,16 @@
         <v>81</v>
       </c>
       <c r="Y60" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z60" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA60" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB60" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC60" s="11" t="s">
         <v>18</v>
@@ -19316,16 +19321,16 @@
         <v>81</v>
       </c>
       <c r="X61" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y61" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z61" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA61" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB61" s="11" t="s">
         <v>18</v>
@@ -19618,16 +19623,16 @@
         <v>81</v>
       </c>
       <c r="X62" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y62" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z62" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA62" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB62" s="11" t="s">
         <v>18</v>
@@ -19774,7 +19779,7 @@
         <v>11</v>
       </c>
       <c r="BX62" s="53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="BY62" s="53" t="s">
         <v>51</v>
@@ -19920,13 +19925,13 @@
         <v>81</v>
       </c>
       <c r="X63" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y63" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z63" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA63" s="11" t="s">
         <v>18</v>
@@ -20219,16 +20224,16 @@
         <v>81</v>
       </c>
       <c r="W64" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X64" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y64" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z64" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA64" s="11" t="s">
         <v>18</v>
@@ -20330,13 +20335,13 @@
         <v>21</v>
       </c>
       <c r="BH64" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BI64" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BJ64" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BK64" s="7" t="s">
         <v>21</v>
@@ -20524,13 +20529,13 @@
         <v>81</v>
       </c>
       <c r="X65" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y65" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z65" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA65" s="11" t="s">
         <v>18</v>
@@ -20632,13 +20637,13 @@
         <v>21</v>
       </c>
       <c r="BH65" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BI65" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BJ65" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BK65" s="7" t="s">
         <v>21</v>
@@ -20826,13 +20831,13 @@
         <v>81</v>
       </c>
       <c r="X66" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y66" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z66" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA66" s="11" t="s">
         <v>18</v>
@@ -20934,13 +20939,13 @@
         <v>21</v>
       </c>
       <c r="BH66" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BI66" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BJ66" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BK66" s="7" t="s">
         <v>21</v>
@@ -21003,7 +21008,7 @@
         <v>47</v>
       </c>
       <c r="CE66" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="CF66" s="20" t="s">
         <v>83</v>
@@ -21134,7 +21139,7 @@
         <v>18</v>
       </c>
       <c r="Z67" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA67" s="11" t="s">
         <v>18</v>
@@ -21308,7 +21313,7 @@
         <v>47</v>
       </c>
       <c r="CF67" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="CG67" s="44" t="s">
         <v>47</v>
@@ -21430,7 +21435,7 @@
         <v>81</v>
       </c>
       <c r="X68" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y68" s="11" t="s">
         <v>18</v>
@@ -21604,13 +21609,13 @@
         <v>11</v>
       </c>
       <c r="CD68" s="44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="CE68" s="44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="CF68" s="44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="CG68" s="44" t="s">
         <v>47</v>
@@ -21732,10 +21737,10 @@
         <v>81</v>
       </c>
       <c r="X69" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y69" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z69" s="10" t="s">
         <v>11</v>
@@ -21906,13 +21911,13 @@
         <v>18</v>
       </c>
       <c r="CD69" s="44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="CE69" s="44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="CF69" s="44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="CG69" s="44" t="s">
         <v>47</v>
@@ -22031,13 +22036,13 @@
         <v>81</v>
       </c>
       <c r="W70" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X70" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y70" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z70" s="10" t="s">
         <v>11</v>
@@ -22327,13 +22332,13 @@
         <v>10</v>
       </c>
       <c r="U71" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V71" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W71" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X71" s="10" t="s">
         <v>11</v>
@@ -22629,13 +22634,13 @@
         <v>10</v>
       </c>
       <c r="U72" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V72" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W72" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X72" s="10" t="s">
         <v>11</v>
@@ -22913,7 +22918,7 @@
         <v>3</v>
       </c>
       <c r="O73" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P73" s="20" t="s">
         <v>10</v>
@@ -22928,10 +22933,10 @@
         <v>10</v>
       </c>
       <c r="T73" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="U73" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V73" s="10" t="s">
         <v>11</v>
@@ -23215,25 +23220,25 @@
         <v>81</v>
       </c>
       <c r="O74" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P74" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q74" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R74" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S74" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T74" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="U74" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V74" s="10" t="s">
         <v>11</v>
@@ -23514,25 +23519,25 @@
         <v>81</v>
       </c>
       <c r="N75" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O75" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P75" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q75" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R75" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S75" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T75" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="U75" s="10" t="s">
         <v>11</v>
@@ -23634,10 +23639,10 @@
         <v>11</v>
       </c>
       <c r="BB75" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BC75" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BD75" s="10" t="s">
         <v>11</v>
@@ -23813,25 +23818,25 @@
         <v>3</v>
       </c>
       <c r="M76" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N76" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O76" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P76" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q76" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R76" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S76" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T76" s="10" t="s">
         <v>11</v>
@@ -23936,10 +23941,10 @@
         <v>11</v>
       </c>
       <c r="BB76" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BC76" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BD76" s="10" t="s">
         <v>11</v>
@@ -24115,7 +24120,7 @@
         <v>81</v>
       </c>
       <c r="M77" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N77" s="43" t="s">
         <v>23</v>
@@ -24127,7 +24132,7 @@
         <v>23</v>
       </c>
       <c r="Q77" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R77" s="10" t="s">
         <v>11</v>
@@ -24414,22 +24419,22 @@
         <v>3</v>
       </c>
       <c r="L78" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M78" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N78" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O78" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P78" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q78" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R78" s="10" t="s">
         <v>11</v>
@@ -24719,22 +24724,22 @@
         <v>3</v>
       </c>
       <c r="M79" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N79" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="O79" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="O79" s="43" t="s">
-        <v>131</v>
-      </c>
       <c r="P79" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q79" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R79" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S79" s="6" t="s">
         <v>5</v>
@@ -24854,7 +24859,7 @@
         <v>18</v>
       </c>
       <c r="BF79" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BG79" s="11" t="s">
         <v>18</v>
@@ -25021,19 +25026,19 @@
         <v>3</v>
       </c>
       <c r="M80" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N80" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O80" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P80" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q80" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R80" s="6" t="s">
         <v>5</v>
@@ -25326,16 +25331,16 @@
         <v>3</v>
       </c>
       <c r="N81" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O81" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P81" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q81" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R81" s="6" t="s">
         <v>5</v>
@@ -25628,13 +25633,13 @@
         <v>3</v>
       </c>
       <c r="N82" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O82" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P82" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q82" s="6" t="s">
         <v>5</v>

</xml_diff>